<commit_message>
Make empty cells with specific types not raise
Previously, if a cell had a type but no value, there would be an xcell
with no 'v' element, causing the spreadsheet to not parse.

Fixes github issue #3
</commit_message>
<xml_diff>
--- a/test/sesame_street_blog.xlsx
+++ b/test/sesame_street_blog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Authors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Formula Dates</t>
+  </si>
+  <si>
+    <t>Empty Eagress</t>
+  </si>
+  <si>
+    <t>The title, date, and comment have types, but no values</t>
   </si>
 </sst>
 </file>
@@ -116,23 +122,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,7 +510,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -578,6 +590,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Empty rows are not generated in the XML
All tests green but the performance is poor.
</commit_message>
<xml_diff>
--- a/test/sesame_street_blog.xlsx
+++ b/test/sesame_street_blog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Authors" sheetId="1" r:id="rId1"/>
     <sheet name="Posts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>The title, date, and comment have types, but no values</t>
+  </si>
+  <si>
+    <t>Small Bird</t>
+  </si>
+  <si>
+    <t>Cleaner</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -496,6 +502,14 @@
       </c>
       <c r="B2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -602,7 +616,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add ability to parse hyperlinks in cells
Previously, if someone put a hyperlink in a URL, we would parse the
"friendly name" and not the URL.

This changes it so that we prioritize parsing the URL, yet don't lose
the "friendly name" if we happen to want it.

PERFORMANCE NOTE: while this does not slow down previous functionality,
spreadsheets with many hyperlinks show to be at least an order of
magnitude slower (maybe two) as well as failing the linear performance
test (which doesn't actually care about overall speed). The performance
test, for now, just tests functionality sans-hyperlinks, but this is an
area that needs improvement.
</commit_message>
<xml_diff>
--- a/test/sesame_street_blog.xlsx
+++ b/test/sesame_street_blog.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woody/Src/in_play/lib/simple_xlsx_reader/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Authors" sheetId="1" r:id="rId1"/>
     <sheet name="Posts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -71,6 +79,12 @@
   </si>
   <si>
     <t>The title, date, and comment have types, but no values</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>This uses the hyperlink GUI option</t>
   </si>
 </sst>
 </file>
@@ -122,7 +136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,25 +144,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -480,9 +502,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -500,28 +522,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -537,8 +554,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -554,8 +574,12 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
+      <c r="F2" s="5" t="str">
+        <f>HYPERLINK("http://www.example.com/hyperlink-function", "This uses the HYPERLINK() function")</f>
+        <v>This uses the HYPERLINK() function</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -571,8 +595,11 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -590,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -601,12 +628,10 @@
       <c r="E5" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>